<commit_message>
figures 3, 4 and 5 updated
</commit_message>
<xml_diff>
--- a/results/supplementary/Table S5. MCMC_model results.xlsx
+++ b/results/supplementary/Table S5. MCMC_model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="11_ED466C965A1253DAD5533D32D96B2AA7ECEDD9E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D83F6B79-DD2D-4780-B473-80461165DF0F}"/>
+  <xr:revisionPtr revIDLastSave="359" documentId="11_ED466C965A1253DAD5533D32D96B2AA7ECEDD9E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90A26D2E-869B-4C4A-A863-0FAEADC12C60}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Lp50 ~ Loil.content</t>
   </si>
   <si>
-    <t>ecology (low vs gen vs alp)</t>
-  </si>
-  <si>
     <t>Loil_content ~ ecology</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>altitudinal preference</t>
   </si>
 </sst>
 </file>
@@ -709,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -770,24 +770,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -836,29 +836,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,7 +1198,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,26 +1219,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="38"/>
+      <c r="A1" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="40"/>
       <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>17</v>
@@ -1267,10 +1262,10 @@
         <v>11</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>10</v>
@@ -1283,138 +1278,138 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="E3" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="31">
+        <v>2.1185160000000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1.4162269999999999</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2.808735</v>
+      </c>
+      <c r="K3" s="1">
+        <v>9576</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="53">
-        <v>2.1185160000000001</v>
-      </c>
-      <c r="I3" s="54">
-        <v>1.4162269999999999</v>
-      </c>
-      <c r="J3" s="54">
-        <v>2.808735</v>
-      </c>
-      <c r="K3" s="54">
-        <v>9576</v>
-      </c>
-      <c r="L3" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="55" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="56" t="s">
+      <c r="H4" s="32">
+        <v>-6.1770000000000002E-3</v>
+      </c>
+      <c r="I4" s="33">
+        <v>-0.26929399999999998</v>
+      </c>
+      <c r="J4" s="33">
+        <v>0.27218999999999999</v>
+      </c>
+      <c r="K4" s="33">
+        <v>9000</v>
+      </c>
+      <c r="L4" s="33">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="M4" s="34"/>
+    </row>
+    <row r="5" spans="1:14" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="56">
-        <v>-6.1770000000000002E-3</v>
-      </c>
-      <c r="I4" s="57">
-        <v>-0.26929399999999998</v>
-      </c>
-      <c r="J4" s="57">
-        <v>0.27218999999999999</v>
-      </c>
-      <c r="K4" s="57">
+      <c r="H5" s="35">
+        <v>-0.104667</v>
+      </c>
+      <c r="I5" s="2">
+        <v>-0.42706499999999997</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.219693</v>
+      </c>
+      <c r="K5" s="2">
         <v>9000</v>
       </c>
-      <c r="L4" s="57">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="M4" s="58"/>
-    </row>
-    <row r="5" spans="1:14" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="59">
-        <v>-0.104667</v>
-      </c>
-      <c r="I5" s="60">
-        <v>-0.42706499999999997</v>
-      </c>
-      <c r="J5" s="60">
-        <v>0.219693</v>
-      </c>
-      <c r="K5" s="60">
-        <v>9000</v>
-      </c>
-      <c r="L5" s="60">
+      <c r="L5" s="2">
         <v>0.50600000000000001</v>
       </c>
-      <c r="M5" s="61"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:14" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="62">
+      <c r="G6" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="36">
         <v>-2.1839999999999998E-2</v>
       </c>
-      <c r="I6" s="63">
+      <c r="I6" s="19">
         <v>-5.9089999999999997E-2</v>
       </c>
-      <c r="J6" s="63">
+      <c r="J6" s="19">
         <v>1.389E-2</v>
       </c>
-      <c r="K6" s="63">
+      <c r="K6" s="19">
         <v>8506</v>
       </c>
-      <c r="L6" s="63">
+      <c r="L6" s="19">
         <v>0.253</v>
       </c>
-      <c r="M6" s="64"/>
+      <c r="M6" s="37"/>
     </row>
     <row r="7" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D7" s="11"/>
@@ -1431,26 +1426,26 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="38"/>
+      <c r="A9" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40"/>
       <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>17</v>
@@ -1474,10 +1469,10 @@
         <v>11</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>10</v>
@@ -1491,25 +1486,25 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H11" s="1">
         <v>-1.9220000000000001E-2</v>
@@ -1530,23 +1525,23 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="31"/>
+        <v>28</v>
+      </c>
+      <c r="B12" s="55"/>
       <c r="C12" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" s="2">
         <v>-1.2959999999999999E-2</v>
@@ -1567,25 +1562,25 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>58</v>
+        <v>33</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>57</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="1">
         <v>-0.72719999999999996</v>
@@ -1603,28 +1598,28 @@
         <v>5.11E-3</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="35"/>
+        <v>34</v>
+      </c>
+      <c r="B14" s="59"/>
       <c r="C14" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" s="2">
         <v>-0.96360000000000001</v>
@@ -1645,25 +1640,25 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>35</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="1">
         <v>2.2499999999999999E-2</v>
@@ -1684,23 +1679,23 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="B16" s="55"/>
       <c r="C16" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="2">
         <v>4.65E-2</v>
@@ -1721,19 +1716,19 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>66</v>
+      <c r="C17" s="56" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>3</v>
@@ -1760,17 +1755,17 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" s="21" t="s">
         <v>3</v>
@@ -1797,19 +1792,19 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>67</v>
+      <c r="C19" s="56" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>3</v>
@@ -1836,17 +1831,17 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>3</v>
@@ -1873,25 +1868,25 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>68</v>
+      <c r="C21" s="56" t="s">
+        <v>67</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21" s="20" t="s">
         <v>3</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="1">
         <v>3.124E-3</v>
@@ -1912,23 +1907,23 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="21" t="s">
         <v>3</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H22" s="2">
         <v>2.0228999999999998E-3</v>
@@ -1946,13 +1941,19 @@
         <v>9.8199999999999996E-2</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A9:M9"/>
@@ -1961,12 +1962,6 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New supplementary with comparison between year of analysis for oil and longevity
</commit_message>
<xml_diff>
--- a/results/supplementary/Table S5. MCMC_model results.xlsx
+++ b/results/supplementary/Table S5. MCMC_model results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/supplementary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="359" documentId="11_ED466C965A1253DAD5533D32D96B2AA7ECEDD9E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90A26D2E-869B-4C4A-A863-0FAEADC12C60}"/>
+  <xr:revisionPtr revIDLastSave="370" documentId="11_ED466C965A1253DAD5533D32D96B2AA7ECEDD9E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941E6458-A90B-4FB8-9857-36C9690AE7C5}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,9 +198,6 @@
     <t>~ animal</t>
   </si>
   <si>
-    <t>p50 (n=37)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Lseedmass ~oilcontent</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>altitudinal preference</t>
+  </si>
+  <si>
+    <t>p50 (n=35)</t>
   </si>
 </sst>
 </file>
@@ -261,6 +261,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -788,6 +789,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -834,24 +853,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -869,10 +870,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1198,7 +1195,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,21 +1216,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1262,10 +1259,10 @@
         <v>11</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>10</v>
@@ -1278,22 +1275,22 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="50" t="s">
+      <c r="C3" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="50" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="30" t="s">
@@ -1319,12 +1316,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="45"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="51"/>
       <c r="G4" s="32" t="s">
         <v>20</v>
       </c>
@@ -1346,12 +1343,12 @@
       <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:14" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="46"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="35" t="s">
         <v>21</v>
       </c>
@@ -1380,10 +1377,10 @@
         <v>23</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>56</v>
@@ -1392,7 +1389,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="36">
         <v>-2.1839999999999998E-2</v>
@@ -1426,21 +1423,21 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="46"/>
       <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,10 +1466,10 @@
         <v>11</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>10</v>
@@ -1488,11 +1485,11 @@
       <c r="A11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="38" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>54</v>
@@ -1504,7 +1501,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="1">
         <v>-1.9220000000000001E-2</v>
@@ -1527,9 +1524,9 @@
       <c r="A12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="55"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>55</v>
@@ -1541,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="2">
         <v>-1.2959999999999999E-2</v>
@@ -1564,11 +1561,11 @@
       <c r="A13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="58" t="s">
-        <v>57</v>
+      <c r="B13" s="42" t="s">
+        <v>69</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -1580,34 +1577,34 @@
         <v>3</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H13" s="1">
-        <v>-0.72719999999999996</v>
+        <v>-0.85070000000000001</v>
       </c>
       <c r="I13" s="1">
-        <v>-1.1793</v>
+        <v>-1.3124</v>
       </c>
       <c r="J13" s="1">
-        <v>-0.26860000000000001</v>
+        <v>-0.39040000000000002</v>
       </c>
       <c r="K13" s="1">
-        <v>9000</v>
+        <v>8483</v>
       </c>
       <c r="L13" s="1">
-        <v>5.11E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="59"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>36</v>
@@ -1619,22 +1616,22 @@
         <v>3</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H14" s="2">
-        <v>-0.96360000000000001</v>
+        <v>-0.73319999999999996</v>
       </c>
       <c r="I14" s="2">
-        <v>-2.5150000000000001</v>
+        <v>-2.2911999999999999</v>
       </c>
       <c r="J14" s="2">
-        <v>0.79</v>
+        <v>1.1489</v>
       </c>
       <c r="K14" s="2">
-        <v>9584</v>
+        <v>9000</v>
       </c>
       <c r="L14" s="2">
-        <v>0.24421999999999999</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="M14" s="4"/>
     </row>
@@ -1642,11 +1639,11 @@
       <c r="A15" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="38" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>37</v>
@@ -1658,7 +1655,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H15" s="1">
         <v>2.2499999999999999E-2</v>
@@ -1681,9 +1678,9 @@
       <c r="A16" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="55"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>38</v>
@@ -1695,7 +1692,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="2">
         <v>4.65E-2</v>
@@ -1721,8 +1718,8 @@
       <c r="B17" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="56" t="s">
-        <v>65</v>
+      <c r="C17" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>45</v>
@@ -1760,7 +1757,7 @@
       <c r="B18" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="57"/>
+      <c r="C18" s="41"/>
       <c r="D18" s="21" t="s">
         <v>46</v>
       </c>
@@ -1797,8 +1794,8 @@
       <c r="B19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="56" t="s">
-        <v>66</v>
+      <c r="C19" s="40" t="s">
+        <v>65</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>49</v>
@@ -1836,7 +1833,7 @@
       <c r="B20" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="57"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="21" t="s">
         <v>50</v>
       </c>
@@ -1873,8 +1870,8 @@
       <c r="B21" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="56" t="s">
-        <v>67</v>
+      <c r="C21" s="40" t="s">
+        <v>66</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>52</v>
@@ -1912,7 +1909,7 @@
       <c r="B22" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="57"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="21" t="s">
         <v>53</v>
       </c>
@@ -1938,22 +1935,16 @@
         <v>9000</v>
       </c>
       <c r="L22" s="2">
-        <v>9.8199999999999996E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A9:M9"/>
@@ -1962,6 +1953,12 @@
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>